<commit_message>
feat(Renombrar_files.ipynb) Al momento de generar los certificados en word, y exportarlo en pdf, tenemos que separarlo por indivdual hay una plataforma que es ilovepdf que lo hace, pero hay una numerativa que se le agrega, entonces mediante este script lo que hace es renombrar los pdf por individual con el nombre del que corresponde, teniendo la data en un excel
</commit_message>
<xml_diff>
--- a/EXCEL_TRABAJADO/2023-1cnl.xlsx
+++ b/EXCEL_TRABAJADO/2023-1cnl.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gians\Desktop\dev\UNDC_AUTOMATIZACION\EXCEL_TRABAJADO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072D2AA6-DA46-47F0-82B3-C8A41FC2501A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B30094C-94BD-4A7F-AA5D-27B5DB733675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{AC3D8E4D-96C0-40C7-9193-949C63F87DF0}"/>
   </bookViews>
@@ -749,8 +749,8 @@
   <dimension ref="A1:K217"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,7 +1227,7 @@
       <c r="B18" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="13" t="s">
         <v>68</v>
       </c>
       <c r="D18" s="24">
@@ -1254,7 +1254,7 @@
       <c r="B19" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="13" t="s">
         <v>68</v>
       </c>
       <c r="D19" s="24">
@@ -1281,7 +1281,7 @@
       <c r="B20" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="13" t="s">
         <v>68</v>
       </c>
       <c r="D20" s="24">
@@ -1308,8 +1308,8 @@
       <c r="B21" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="24" t="s">
-        <v>44</v>
+      <c r="C21" s="13" t="s">
+        <v>68</v>
       </c>
       <c r="D21" s="24">
         <v>4</v>
@@ -2352,7 +2352,7 @@
         <v>6</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -2364,10 +2364,10 @@
         <v>34</v>
       </c>
       <c r="G60" s="2">
-        <v>0.5</v>
+        <v>0.65625</v>
       </c>
       <c r="H60" s="2">
-        <v>0.625</v>
+        <v>0.75</v>
       </c>
       <c r="K60" s="1"/>
     </row>
@@ -2379,7 +2379,7 @@
         <v>6</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -2406,7 +2406,7 @@
         <v>6</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -2421,7 +2421,7 @@
         <v>0.75</v>
       </c>
       <c r="H62" s="2">
-        <v>0.84375</v>
+        <v>0.8125</v>
       </c>
       <c r="K62" s="1"/>
     </row>
@@ -2433,7 +2433,7 @@
         <v>6</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -2442,13 +2442,13 @@
         <v>16</v>
       </c>
       <c r="F63" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G63" s="2">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="H63" s="2">
-        <v>0.84375</v>
+        <v>0.65625</v>
       </c>
       <c r="K63" s="1"/>
     </row>
@@ -3890,7 +3890,7 @@
       <c r="B117" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C117" s="17" t="s">
+      <c r="C117" s="13" t="s">
         <v>68</v>
       </c>
       <c r="D117" s="17">
@@ -3917,7 +3917,7 @@
       <c r="B118" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C118" s="17" t="s">
+      <c r="C118" s="13" t="s">
         <v>68</v>
       </c>
       <c r="D118" s="17">
@@ -3944,7 +3944,7 @@
       <c r="B119" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C119" s="17" t="s">
+      <c r="C119" s="13" t="s">
         <v>68</v>
       </c>
       <c r="D119" s="17">
@@ -3971,7 +3971,7 @@
       <c r="B120" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C120" s="17" t="s">
+      <c r="C120" s="13" t="s">
         <v>68</v>
       </c>
       <c r="D120" s="17">
@@ -3998,7 +3998,7 @@
       <c r="B121" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C121" s="17" t="s">
+      <c r="C121" s="13" t="s">
         <v>68</v>
       </c>
       <c r="D121" s="17">
@@ -4025,7 +4025,7 @@
       <c r="B122" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C122" s="17" t="s">
+      <c r="C122" s="13" t="s">
         <v>68</v>
       </c>
       <c r="D122" s="17">

</xml_diff>

<commit_message>
[FIX] change tag whatsapp bussiness
</commit_message>
<xml_diff>
--- a/EXCEL_TRABAJADO/2023-1cnl.xlsx
+++ b/EXCEL_TRABAJADO/2023-1cnl.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gians\Desktop\dev\UNDC_AUTOMATIZACION\EXCEL_TRABAJADO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B30094C-94BD-4A7F-AA5D-27B5DB733675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD90550C-342E-43B9-93D6-33FC3D77C891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{AC3D8E4D-96C0-40C7-9193-949C63F87DF0}"/>
   </bookViews>
@@ -749,8 +749,8 @@
   <dimension ref="A1:K217"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H57" sqref="H57"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,10 +799,10 @@
         <v>68</v>
       </c>
       <c r="D2" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E2" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>35</v>
@@ -826,10 +826,10 @@
         <v>68</v>
       </c>
       <c r="D3" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E3" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>35</v>
@@ -853,10 +853,10 @@
         <v>68</v>
       </c>
       <c r="D4" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E4" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>40</v>
@@ -880,10 +880,10 @@
         <v>68</v>
       </c>
       <c r="D5" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E5" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>40</v>
@@ -907,10 +907,10 @@
         <v>68</v>
       </c>
       <c r="D6" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E6" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>40</v>
@@ -934,10 +934,10 @@
         <v>68</v>
       </c>
       <c r="D7" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E7" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>38</v>
@@ -960,11 +960,11 @@
       <c r="C8" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>16</v>
+      <c r="D8" s="13">
+        <v>17</v>
+      </c>
+      <c r="E8" s="13">
+        <v>18</v>
       </c>
       <c r="F8" t="s">
         <v>34</v>
@@ -987,11 +987,11 @@
       <c r="C9" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>16</v>
+      <c r="D9" s="13">
+        <v>17</v>
+      </c>
+      <c r="E9" s="13">
+        <v>18</v>
       </c>
       <c r="F9" t="s">
         <v>39</v>
@@ -1014,11 +1014,11 @@
       <c r="C10" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>16</v>
+      <c r="D10" s="13">
+        <v>17</v>
+      </c>
+      <c r="E10" s="13">
+        <v>18</v>
       </c>
       <c r="F10" t="s">
         <v>35</v>
@@ -1041,11 +1041,11 @@
       <c r="C11" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>16</v>
+      <c r="D11" s="13">
+        <v>17</v>
+      </c>
+      <c r="E11" s="13">
+        <v>18</v>
       </c>
       <c r="F11" t="s">
         <v>36</v>
@@ -1068,11 +1068,11 @@
       <c r="C12" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>16</v>
+      <c r="D12" s="13">
+        <v>17</v>
+      </c>
+      <c r="E12" s="13">
+        <v>18</v>
       </c>
       <c r="F12" t="s">
         <v>40</v>
@@ -1096,10 +1096,10 @@
         <v>68</v>
       </c>
       <c r="D13" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E13" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F13" s="13" t="s">
         <v>34</v>
@@ -1123,10 +1123,10 @@
         <v>68</v>
       </c>
       <c r="D14" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E14" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F14" s="13" t="s">
         <v>39</v>
@@ -1150,10 +1150,10 @@
         <v>68</v>
       </c>
       <c r="D15" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E15" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F15" s="13" t="s">
         <v>35</v>
@@ -1177,10 +1177,10 @@
         <v>68</v>
       </c>
       <c r="D16" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E16" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F16" s="13" t="s">
         <v>36</v>
@@ -1204,10 +1204,10 @@
         <v>68</v>
       </c>
       <c r="D17" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E17" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F17" s="13" t="s">
         <v>40</v>
@@ -1230,11 +1230,11 @@
       <c r="C18" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D18" s="24">
-        <v>2</v>
-      </c>
-      <c r="E18" s="24">
-        <v>16</v>
+      <c r="D18" s="13">
+        <v>17</v>
+      </c>
+      <c r="E18" s="13">
+        <v>18</v>
       </c>
       <c r="F18" s="24" t="s">
         <v>34</v>
@@ -1257,11 +1257,11 @@
       <c r="C19" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="24">
-        <v>1</v>
-      </c>
-      <c r="E19" s="24">
-        <v>16</v>
+      <c r="D19" s="13">
+        <v>17</v>
+      </c>
+      <c r="E19" s="13">
+        <v>18</v>
       </c>
       <c r="F19" s="24" t="s">
         <v>35</v>
@@ -1284,11 +1284,11 @@
       <c r="C20" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="24">
-        <v>1</v>
-      </c>
-      <c r="E20" s="24">
-        <v>16</v>
+      <c r="D20" s="13">
+        <v>17</v>
+      </c>
+      <c r="E20" s="13">
+        <v>18</v>
       </c>
       <c r="F20" s="24" t="s">
         <v>40</v>
@@ -1311,11 +1311,11 @@
       <c r="C21" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="24">
-        <v>4</v>
-      </c>
-      <c r="E21" s="24">
-        <v>4</v>
+      <c r="D21" s="13">
+        <v>17</v>
+      </c>
+      <c r="E21" s="13">
+        <v>18</v>
       </c>
       <c r="F21" s="24" t="s">
         <v>38</v>
@@ -1338,11 +1338,11 @@
       <c r="C22" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="23">
-        <v>1</v>
-      </c>
-      <c r="E22" s="23">
-        <v>16</v>
+      <c r="D22" s="13">
+        <v>17</v>
+      </c>
+      <c r="E22" s="13">
+        <v>18</v>
       </c>
       <c r="F22" s="23" t="s">
         <v>39</v>
@@ -1365,11 +1365,11 @@
       <c r="C23" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="23">
-        <v>1</v>
-      </c>
-      <c r="E23" s="23">
-        <v>16</v>
+      <c r="D23" s="13">
+        <v>17</v>
+      </c>
+      <c r="E23" s="13">
+        <v>18</v>
       </c>
       <c r="F23" s="23" t="s">
         <v>39</v>
@@ -1393,10 +1393,10 @@
         <v>68</v>
       </c>
       <c r="D24" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E24" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F24" s="13" t="s">
         <v>35</v>
@@ -1420,10 +1420,10 @@
         <v>68</v>
       </c>
       <c r="D25" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E25" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F25" s="13" t="s">
         <v>36</v>
@@ -1447,10 +1447,10 @@
         <v>68</v>
       </c>
       <c r="D26" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E26" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F26" s="13" t="s">
         <v>40</v>
@@ -1473,11 +1473,11 @@
       <c r="C27" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>16</v>
+      <c r="D27" s="13">
+        <v>17</v>
+      </c>
+      <c r="E27" s="13">
+        <v>18</v>
       </c>
       <c r="F27" t="s">
         <v>34</v>
@@ -1500,11 +1500,11 @@
       <c r="C28" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28">
-        <v>16</v>
+      <c r="D28" s="13">
+        <v>17</v>
+      </c>
+      <c r="E28" s="13">
+        <v>18</v>
       </c>
       <c r="F28" t="s">
         <v>39</v>
@@ -1527,11 +1527,11 @@
       <c r="C29" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29">
-        <v>16</v>
+      <c r="D29" s="13">
+        <v>17</v>
+      </c>
+      <c r="E29" s="13">
+        <v>18</v>
       </c>
       <c r="F29" t="s">
         <v>39</v>
@@ -1554,11 +1554,11 @@
       <c r="C30" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30">
-        <v>16</v>
+      <c r="D30" s="13">
+        <v>17</v>
+      </c>
+      <c r="E30" s="13">
+        <v>18</v>
       </c>
       <c r="F30" t="s">
         <v>39</v>
@@ -1581,11 +1581,11 @@
       <c r="C31" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31">
-        <v>16</v>
+      <c r="D31" s="13">
+        <v>17</v>
+      </c>
+      <c r="E31" s="13">
+        <v>18</v>
       </c>
       <c r="F31" t="s">
         <v>39</v>
@@ -1608,11 +1608,11 @@
       <c r="C32" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32">
-        <v>16</v>
+      <c r="D32" s="13">
+        <v>17</v>
+      </c>
+      <c r="E32" s="13">
+        <v>18</v>
       </c>
       <c r="F32" t="s">
         <v>39</v>
@@ -1635,11 +1635,11 @@
       <c r="C33" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33">
-        <v>16</v>
+      <c r="D33" s="13">
+        <v>17</v>
+      </c>
+      <c r="E33" s="13">
+        <v>18</v>
       </c>
       <c r="F33" t="s">
         <v>35</v>
@@ -1662,8 +1662,12 @@
       <c r="C34" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
+      <c r="D34" s="13">
+        <v>17</v>
+      </c>
+      <c r="E34" s="13">
+        <v>18</v>
+      </c>
       <c r="F34" s="17"/>
       <c r="G34" s="19"/>
       <c r="H34" s="19"/>
@@ -1677,13 +1681,13 @@
         <v>65</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D35" s="13">
+        <v>17</v>
+      </c>
+      <c r="E35" s="13">
+        <v>18</v>
       </c>
       <c r="F35" t="s">
         <v>35</v>
@@ -1704,13 +1708,13 @@
         <v>65</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D36" s="13">
+        <v>17</v>
+      </c>
+      <c r="E36" s="13">
+        <v>18</v>
       </c>
       <c r="F36" t="s">
         <v>36</v>
@@ -1731,13 +1735,13 @@
         <v>65</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D37" s="13">
+        <v>17</v>
+      </c>
+      <c r="E37" s="13">
+        <v>18</v>
       </c>
       <c r="F37" t="s">
         <v>40</v>
@@ -1758,13 +1762,13 @@
         <v>65</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D38" s="13">
+        <v>17</v>
+      </c>
+      <c r="E38" s="13">
+        <v>18</v>
       </c>
       <c r="F38" t="s">
         <v>40</v>
@@ -1785,13 +1789,13 @@
         <v>65</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D39" s="13">
+        <v>17</v>
+      </c>
+      <c r="E39" s="13">
+        <v>18</v>
       </c>
       <c r="F39" t="s">
         <v>38</v>
@@ -1812,13 +1816,13 @@
         <v>65</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="E40">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D40" s="13">
+        <v>17</v>
+      </c>
+      <c r="E40" s="13">
+        <v>18</v>
       </c>
       <c r="F40" t="s">
         <v>38</v>
@@ -1839,13 +1843,13 @@
         <v>64</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D41" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E41" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F41" s="13" t="s">
         <v>39</v>
@@ -1866,13 +1870,13 @@
         <v>64</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D42" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E42" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F42" s="13" t="s">
         <v>35</v>
@@ -1893,13 +1897,13 @@
         <v>64</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D43" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E43" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F43" s="13" t="s">
         <v>35</v>
@@ -1920,13 +1924,13 @@
         <v>64</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D44" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E44" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F44" s="13" t="s">
         <v>36</v>
@@ -1947,13 +1951,13 @@
         <v>24</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-      <c r="E45">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D45" s="13">
+        <v>17</v>
+      </c>
+      <c r="E45" s="13">
+        <v>18</v>
       </c>
       <c r="F45" t="s">
         <v>34</v>
@@ -1974,13 +1978,13 @@
         <v>24</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-      <c r="E46">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D46" s="13">
+        <v>17</v>
+      </c>
+      <c r="E46" s="13">
+        <v>18</v>
       </c>
       <c r="F46" t="s">
         <v>39</v>
@@ -2001,13 +2005,13 @@
         <v>24</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-      <c r="E47">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D47" s="13">
+        <v>17</v>
+      </c>
+      <c r="E47" s="13">
+        <v>18</v>
       </c>
       <c r="F47" t="s">
         <v>39</v>
@@ -2028,13 +2032,13 @@
         <v>24</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D48">
-        <v>1</v>
-      </c>
-      <c r="E48">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D48" s="13">
+        <v>17</v>
+      </c>
+      <c r="E48" s="13">
+        <v>18</v>
       </c>
       <c r="F48" t="s">
         <v>35</v>
@@ -2055,13 +2059,13 @@
         <v>24</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-      <c r="E49">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D49" s="13">
+        <v>17</v>
+      </c>
+      <c r="E49" s="13">
+        <v>18</v>
       </c>
       <c r="F49" t="s">
         <v>35</v>
@@ -2082,13 +2086,13 @@
         <v>24</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D50">
-        <v>1</v>
-      </c>
-      <c r="E50">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D50" s="13">
+        <v>17</v>
+      </c>
+      <c r="E50" s="13">
+        <v>18</v>
       </c>
       <c r="F50" t="s">
         <v>36</v>
@@ -2109,13 +2113,13 @@
         <v>24</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D51">
-        <v>1</v>
-      </c>
-      <c r="E51">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D51" s="13">
+        <v>17</v>
+      </c>
+      <c r="E51" s="13">
+        <v>18</v>
       </c>
       <c r="F51" t="s">
         <v>40</v>
@@ -2136,13 +2140,13 @@
         <v>14</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D52" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E52" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F52" s="13" t="s">
         <v>34</v>
@@ -2163,13 +2167,13 @@
         <v>14</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D53" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E53" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F53" s="13" t="s">
         <v>39</v>
@@ -2190,13 +2194,13 @@
         <v>14</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D54" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E54" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F54" s="13" t="s">
         <v>35</v>
@@ -2217,13 +2221,13 @@
         <v>14</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D55" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E55" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F55" s="13" t="s">
         <v>38</v>
@@ -2244,13 +2248,13 @@
         <v>22</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D56">
-        <v>7</v>
-      </c>
-      <c r="E56">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D56" s="13">
+        <v>17</v>
+      </c>
+      <c r="E56" s="13">
+        <v>18</v>
       </c>
       <c r="F56" t="s">
         <v>39</v>
@@ -2271,13 +2275,13 @@
         <v>22</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D57">
-        <v>7</v>
-      </c>
-      <c r="E57">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D57" s="13">
+        <v>17</v>
+      </c>
+      <c r="E57" s="13">
+        <v>18</v>
       </c>
       <c r="F57" t="s">
         <v>35</v>
@@ -2298,13 +2302,13 @@
         <v>22</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D58">
-        <v>7</v>
-      </c>
-      <c r="E58">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D58" s="13">
+        <v>17</v>
+      </c>
+      <c r="E58" s="13">
+        <v>18</v>
       </c>
       <c r="F58" t="s">
         <v>35</v>
@@ -2325,13 +2329,13 @@
         <v>22</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D59">
-        <v>7</v>
-      </c>
-      <c r="E59">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D59" s="13">
+        <v>17</v>
+      </c>
+      <c r="E59" s="13">
+        <v>18</v>
       </c>
       <c r="F59" t="s">
         <v>40</v>
@@ -2351,14 +2355,14 @@
       <c r="B60" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C60" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D60">
-        <v>1</v>
-      </c>
-      <c r="E60">
-        <v>16</v>
+      <c r="C60" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D60" s="13">
+        <v>17</v>
+      </c>
+      <c r="E60" s="13">
+        <v>18</v>
       </c>
       <c r="F60" t="s">
         <v>34</v>
@@ -2378,14 +2382,14 @@
       <c r="B61" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C61" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D61">
-        <v>1</v>
-      </c>
-      <c r="E61">
-        <v>16</v>
+      <c r="C61" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D61" s="13">
+        <v>17</v>
+      </c>
+      <c r="E61" s="13">
+        <v>18</v>
       </c>
       <c r="F61" t="s">
         <v>34</v>
@@ -2405,14 +2409,14 @@
       <c r="B62" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C62" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D62">
-        <v>1</v>
-      </c>
-      <c r="E62">
-        <v>16</v>
+      <c r="C62" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D62" s="13">
+        <v>17</v>
+      </c>
+      <c r="E62" s="13">
+        <v>18</v>
       </c>
       <c r="F62" t="s">
         <v>39</v>
@@ -2432,14 +2436,14 @@
       <c r="B63" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C63" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D63">
-        <v>1</v>
-      </c>
-      <c r="E63">
-        <v>16</v>
+      <c r="C63" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D63" s="13">
+        <v>17</v>
+      </c>
+      <c r="E63" s="13">
+        <v>18</v>
       </c>
       <c r="F63" t="s">
         <v>35</v>
@@ -2460,13 +2464,13 @@
         <v>4</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D64" s="9">
-        <v>1</v>
-      </c>
-      <c r="E64" s="9">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D64" s="13">
+        <v>17</v>
+      </c>
+      <c r="E64" s="13">
+        <v>18</v>
       </c>
       <c r="F64" s="9" t="s">
         <v>39</v>
@@ -2487,13 +2491,13 @@
         <v>4</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D65" s="9">
-        <v>1</v>
-      </c>
-      <c r="E65" s="9">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D65" s="13">
+        <v>17</v>
+      </c>
+      <c r="E65" s="13">
+        <v>18</v>
       </c>
       <c r="F65" s="9" t="s">
         <v>34</v>
@@ -2514,13 +2518,13 @@
         <v>4</v>
       </c>
       <c r="C66" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D66" s="9">
-        <v>1</v>
-      </c>
-      <c r="E66" s="9">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D66" s="13">
+        <v>17</v>
+      </c>
+      <c r="E66" s="13">
+        <v>18</v>
       </c>
       <c r="F66" s="9" t="s">
         <v>35</v>
@@ -2541,13 +2545,13 @@
         <v>4</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D67" s="9">
-        <v>1</v>
-      </c>
-      <c r="E67" s="9">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D67" s="13">
+        <v>17</v>
+      </c>
+      <c r="E67" s="13">
+        <v>18</v>
       </c>
       <c r="F67" s="9" t="s">
         <v>36</v>
@@ -2568,13 +2572,13 @@
         <v>4</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D68" s="9">
-        <v>1</v>
-      </c>
-      <c r="E68" s="9">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D68" s="13">
+        <v>17</v>
+      </c>
+      <c r="E68" s="13">
+        <v>18</v>
       </c>
       <c r="F68" s="9" t="s">
         <v>40</v>
@@ -2595,13 +2599,13 @@
         <v>4</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D69" s="9">
-        <v>1</v>
-      </c>
-      <c r="E69" s="9">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D69" s="13">
+        <v>17</v>
+      </c>
+      <c r="E69" s="13">
+        <v>18</v>
       </c>
       <c r="F69" s="9" t="s">
         <v>39</v>
@@ -2622,13 +2626,13 @@
         <v>4</v>
       </c>
       <c r="C70" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D70" s="9">
-        <v>1</v>
-      </c>
-      <c r="E70" s="9">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D70" s="13">
+        <v>17</v>
+      </c>
+      <c r="E70" s="13">
+        <v>18</v>
       </c>
       <c r="F70" s="9" t="s">
         <v>35</v>
@@ -2649,13 +2653,13 @@
         <v>4</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D71" s="9">
-        <v>1</v>
-      </c>
-      <c r="E71" s="9">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D71" s="13">
+        <v>17</v>
+      </c>
+      <c r="E71" s="13">
+        <v>18</v>
       </c>
       <c r="F71" s="9" t="s">
         <v>35</v>
@@ -2676,13 +2680,13 @@
         <v>4</v>
       </c>
       <c r="C72" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D72" s="9">
-        <v>1</v>
-      </c>
-      <c r="E72" s="9">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D72" s="13">
+        <v>17</v>
+      </c>
+      <c r="E72" s="13">
+        <v>18</v>
       </c>
       <c r="F72" s="9" t="s">
         <v>39</v>
@@ -2703,13 +2707,13 @@
         <v>4</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D73" s="9">
-        <v>1</v>
-      </c>
-      <c r="E73" s="9">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D73" s="13">
+        <v>17</v>
+      </c>
+      <c r="E73" s="13">
+        <v>18</v>
       </c>
       <c r="F73" s="9" t="s">
         <v>35</v>
@@ -2730,13 +2734,13 @@
         <v>4</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D74" s="9">
-        <v>1</v>
-      </c>
-      <c r="E74" s="9">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D74" s="13">
+        <v>17</v>
+      </c>
+      <c r="E74" s="13">
+        <v>18</v>
       </c>
       <c r="F74" s="9" t="s">
         <v>36</v>
@@ -2757,13 +2761,13 @@
         <v>4</v>
       </c>
       <c r="C75" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D75" s="9">
-        <v>1</v>
-      </c>
-      <c r="E75" s="9">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D75" s="13">
+        <v>17</v>
+      </c>
+      <c r="E75" s="13">
+        <v>18</v>
       </c>
       <c r="F75" s="9" t="s">
         <v>40</v>
@@ -2784,13 +2788,13 @@
         <v>4</v>
       </c>
       <c r="C76" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D76" s="9">
-        <v>1</v>
-      </c>
-      <c r="E76" s="9">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D76" s="13">
+        <v>17</v>
+      </c>
+      <c r="E76" s="13">
+        <v>18</v>
       </c>
       <c r="F76" s="9" t="s">
         <v>40</v>
@@ -2811,13 +2815,13 @@
         <v>58</v>
       </c>
       <c r="C77" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D77">
-        <v>1</v>
-      </c>
-      <c r="E77">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D77" s="13">
+        <v>17</v>
+      </c>
+      <c r="E77" s="13">
+        <v>18</v>
       </c>
       <c r="F77" t="s">
         <v>35</v>
@@ -2838,13 +2842,13 @@
         <v>58</v>
       </c>
       <c r="C78" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D78">
-        <v>1</v>
-      </c>
-      <c r="E78">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D78" s="13">
+        <v>17</v>
+      </c>
+      <c r="E78" s="13">
+        <v>18</v>
       </c>
       <c r="F78" t="s">
         <v>35</v>
@@ -2865,13 +2869,13 @@
         <v>58</v>
       </c>
       <c r="C79" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D79">
-        <v>1</v>
-      </c>
-      <c r="E79">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D79" s="13">
+        <v>17</v>
+      </c>
+      <c r="E79" s="13">
+        <v>18</v>
       </c>
       <c r="F79" t="s">
         <v>36</v>
@@ -2892,13 +2896,13 @@
         <v>58</v>
       </c>
       <c r="C80" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D80">
-        <v>1</v>
-      </c>
-      <c r="E80">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D80" s="13">
+        <v>17</v>
+      </c>
+      <c r="E80" s="13">
+        <v>18</v>
       </c>
       <c r="F80" t="s">
         <v>40</v>
@@ -2919,13 +2923,13 @@
         <v>62</v>
       </c>
       <c r="C81" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D81" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E81" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F81" s="13" t="s">
         <v>34</v>
@@ -2946,13 +2950,13 @@
         <v>62</v>
       </c>
       <c r="C82" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D82" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E82" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F82" s="13" t="s">
         <v>34</v>
@@ -2973,13 +2977,13 @@
         <v>62</v>
       </c>
       <c r="C83" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D83" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E83" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F83" s="13" t="s">
         <v>35</v>
@@ -3000,13 +3004,13 @@
         <v>62</v>
       </c>
       <c r="C84" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D84" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E84" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F84" s="13" t="s">
         <v>36</v>
@@ -3027,13 +3031,13 @@
         <v>10</v>
       </c>
       <c r="C85" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D85">
-        <v>1</v>
-      </c>
-      <c r="E85">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D85" s="13">
+        <v>17</v>
+      </c>
+      <c r="E85" s="13">
+        <v>18</v>
       </c>
       <c r="F85" t="s">
         <v>34</v>
@@ -3054,13 +3058,13 @@
         <v>10</v>
       </c>
       <c r="C86" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D86">
-        <v>1</v>
-      </c>
-      <c r="E86">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D86" s="13">
+        <v>17</v>
+      </c>
+      <c r="E86" s="13">
+        <v>18</v>
       </c>
       <c r="F86" t="s">
         <v>34</v>
@@ -3081,13 +3085,13 @@
         <v>10</v>
       </c>
       <c r="C87" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D87">
-        <v>1</v>
-      </c>
-      <c r="E87">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D87" s="13">
+        <v>17</v>
+      </c>
+      <c r="E87" s="13">
+        <v>18</v>
       </c>
       <c r="F87" t="s">
         <v>34</v>
@@ -3108,13 +3112,13 @@
         <v>10</v>
       </c>
       <c r="C88" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D88">
-        <v>1</v>
-      </c>
-      <c r="E88">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D88" s="13">
+        <v>17</v>
+      </c>
+      <c r="E88" s="13">
+        <v>18</v>
       </c>
       <c r="F88" t="s">
         <v>39</v>
@@ -3135,13 +3139,13 @@
         <v>10</v>
       </c>
       <c r="C89" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D89">
-        <v>1</v>
-      </c>
-      <c r="E89">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D89" s="13">
+        <v>17</v>
+      </c>
+      <c r="E89" s="13">
+        <v>18</v>
       </c>
       <c r="F89" t="s">
         <v>39</v>
@@ -3162,13 +3166,13 @@
         <v>10</v>
       </c>
       <c r="C90" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D90">
-        <v>1</v>
-      </c>
-      <c r="E90">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D90" s="13">
+        <v>17</v>
+      </c>
+      <c r="E90" s="13">
+        <v>18</v>
       </c>
       <c r="F90" t="s">
         <v>35</v>
@@ -3189,13 +3193,13 @@
         <v>10</v>
       </c>
       <c r="C91" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D91">
-        <v>1</v>
-      </c>
-      <c r="E91">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D91" s="13">
+        <v>17</v>
+      </c>
+      <c r="E91" s="13">
+        <v>18</v>
       </c>
       <c r="F91" t="s">
         <v>35</v>
@@ -3216,13 +3220,13 @@
         <v>10</v>
       </c>
       <c r="C92" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D92">
-        <v>1</v>
-      </c>
-      <c r="E92">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D92" s="13">
+        <v>17</v>
+      </c>
+      <c r="E92" s="13">
+        <v>18</v>
       </c>
       <c r="F92" t="s">
         <v>36</v>
@@ -3243,13 +3247,13 @@
         <v>67</v>
       </c>
       <c r="C93" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D93" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E93" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F93" s="13" t="s">
         <v>34</v>
@@ -3270,13 +3274,13 @@
         <v>67</v>
       </c>
       <c r="C94" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D94" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E94" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F94" s="13" t="s">
         <v>36</v>
@@ -3297,13 +3301,13 @@
         <v>67</v>
       </c>
       <c r="C95" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D95" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E95" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F95" s="13" t="s">
         <v>38</v>
@@ -3324,13 +3328,13 @@
         <v>66</v>
       </c>
       <c r="C96" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D96" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E96" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F96" s="13" t="s">
         <v>39</v>
@@ -3351,13 +3355,13 @@
         <v>66</v>
       </c>
       <c r="C97" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D97" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E97" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F97" s="13" t="s">
         <v>38</v>
@@ -3378,13 +3382,13 @@
         <v>28</v>
       </c>
       <c r="C98" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D98" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E98" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F98" s="13" t="s">
         <v>36</v>
@@ -3405,13 +3409,13 @@
         <v>28</v>
       </c>
       <c r="C99" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D99" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E99" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F99" s="13" t="s">
         <v>36</v>
@@ -3432,13 +3436,13 @@
         <v>28</v>
       </c>
       <c r="C100" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D100" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E100" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F100" s="13" t="s">
         <v>40</v>
@@ -3459,13 +3463,13 @@
         <v>28</v>
       </c>
       <c r="C101" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D101" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E101" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F101" s="13" t="s">
         <v>40</v>
@@ -3486,13 +3490,13 @@
         <v>28</v>
       </c>
       <c r="C102" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D102" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E102" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F102" s="13" t="s">
         <v>40</v>
@@ -3513,13 +3517,13 @@
         <v>28</v>
       </c>
       <c r="C103" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D103" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E103" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F103" s="13" t="s">
         <v>38</v>
@@ -3540,13 +3544,13 @@
         <v>59</v>
       </c>
       <c r="C104" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D104">
-        <v>1</v>
-      </c>
-      <c r="E104">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D104" s="13">
+        <v>17</v>
+      </c>
+      <c r="E104" s="13">
+        <v>18</v>
       </c>
       <c r="F104" t="s">
         <v>34</v>
@@ -3567,13 +3571,13 @@
         <v>59</v>
       </c>
       <c r="C105" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D105">
-        <v>1</v>
-      </c>
-      <c r="E105">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D105" s="13">
+        <v>17</v>
+      </c>
+      <c r="E105" s="13">
+        <v>18</v>
       </c>
       <c r="F105" t="s">
         <v>34</v>
@@ -3594,13 +3598,13 @@
         <v>59</v>
       </c>
       <c r="C106" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D106">
-        <v>1</v>
-      </c>
-      <c r="E106">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D106" s="13">
+        <v>17</v>
+      </c>
+      <c r="E106" s="13">
+        <v>18</v>
       </c>
       <c r="F106" t="s">
         <v>36</v>
@@ -3621,13 +3625,13 @@
         <v>26</v>
       </c>
       <c r="C107" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D107" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E107" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F107" s="13" t="s">
         <v>34</v>
@@ -3648,13 +3652,13 @@
         <v>26</v>
       </c>
       <c r="C108" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D108" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E108" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F108" s="13" t="s">
         <v>34</v>
@@ -3675,13 +3679,13 @@
         <v>26</v>
       </c>
       <c r="C109" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D109" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E109" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F109" s="13" t="s">
         <v>34</v>
@@ -3702,13 +3706,13 @@
         <v>26</v>
       </c>
       <c r="C110" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D110" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E110" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F110" s="13" t="s">
         <v>39</v>
@@ -3729,13 +3733,13 @@
         <v>26</v>
       </c>
       <c r="C111" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D111" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E111" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F111" s="13" t="s">
         <v>35</v>
@@ -3756,13 +3760,13 @@
         <v>26</v>
       </c>
       <c r="C112" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D112" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E112" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F112" s="13" t="s">
         <v>35</v>
@@ -3783,13 +3787,13 @@
         <v>26</v>
       </c>
       <c r="C113" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D113" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E113" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F113" s="13" t="s">
         <v>35</v>
@@ -3810,13 +3814,13 @@
         <v>26</v>
       </c>
       <c r="C114" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D114" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E114" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F114" s="13" t="s">
         <v>35</v>
@@ -3837,13 +3841,13 @@
         <v>26</v>
       </c>
       <c r="C115" s="13" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D115" s="13">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E115" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F115" s="13" t="s">
         <v>40</v>
@@ -3864,13 +3868,13 @@
         <v>8</v>
       </c>
       <c r="C116" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D116">
-        <v>1</v>
-      </c>
-      <c r="E116">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D116" s="13">
+        <v>17</v>
+      </c>
+      <c r="E116" s="13">
+        <v>18</v>
       </c>
       <c r="F116" t="s">
         <v>36</v>
@@ -3891,13 +3895,13 @@
         <v>18</v>
       </c>
       <c r="C117" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D117" s="17">
-        <v>1</v>
-      </c>
-      <c r="E117" s="17">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D117" s="13">
+        <v>17</v>
+      </c>
+      <c r="E117" s="13">
+        <v>18</v>
       </c>
       <c r="F117" s="17" t="s">
         <v>34</v>
@@ -3918,13 +3922,13 @@
         <v>18</v>
       </c>
       <c r="C118" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D118" s="17">
-        <v>1</v>
-      </c>
-      <c r="E118" s="17">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D118" s="13">
+        <v>17</v>
+      </c>
+      <c r="E118" s="13">
+        <v>18</v>
       </c>
       <c r="F118" s="17" t="s">
         <v>34</v>
@@ -3945,13 +3949,13 @@
         <v>18</v>
       </c>
       <c r="C119" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D119" s="17">
-        <v>1</v>
-      </c>
-      <c r="E119" s="17">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D119" s="13">
+        <v>17</v>
+      </c>
+      <c r="E119" s="13">
+        <v>18</v>
       </c>
       <c r="F119" s="17" t="s">
         <v>35</v>
@@ -3972,13 +3976,13 @@
         <v>18</v>
       </c>
       <c r="C120" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D120" s="17">
-        <v>1</v>
-      </c>
-      <c r="E120" s="17">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D120" s="13">
+        <v>17</v>
+      </c>
+      <c r="E120" s="13">
+        <v>18</v>
       </c>
       <c r="F120" s="17" t="s">
         <v>35</v>
@@ -3999,13 +4003,13 @@
         <v>18</v>
       </c>
       <c r="C121" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D121" s="17">
-        <v>1</v>
-      </c>
-      <c r="E121" s="17">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D121" s="13">
+        <v>17</v>
+      </c>
+      <c r="E121" s="13">
+        <v>18</v>
       </c>
       <c r="F121" s="17" t="s">
         <v>36</v>
@@ -4026,13 +4030,13 @@
         <v>18</v>
       </c>
       <c r="C122" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D122" s="17">
-        <v>1</v>
-      </c>
-      <c r="E122" s="17">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D122" s="13">
+        <v>17</v>
+      </c>
+      <c r="E122" s="13">
+        <v>18</v>
       </c>
       <c r="F122" s="17" t="s">
         <v>40</v>
@@ -4053,13 +4057,13 @@
         <v>16</v>
       </c>
       <c r="C123" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D123">
-        <v>1</v>
-      </c>
-      <c r="E123">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D123" s="13">
+        <v>17</v>
+      </c>
+      <c r="E123" s="13">
+        <v>18</v>
       </c>
       <c r="F123" t="s">
         <v>38</v>
@@ -4080,13 +4084,13 @@
         <v>16</v>
       </c>
       <c r="C124" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D124">
-        <v>1</v>
-      </c>
-      <c r="E124">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D124" s="13">
+        <v>17</v>
+      </c>
+      <c r="E124" s="13">
+        <v>18</v>
       </c>
       <c r="F124" t="s">
         <v>38</v>
@@ -4107,13 +4111,13 @@
         <v>16</v>
       </c>
       <c r="C125" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D125">
-        <v>1</v>
-      </c>
-      <c r="E125">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D125" s="13">
+        <v>17</v>
+      </c>
+      <c r="E125" s="13">
+        <v>18</v>
       </c>
       <c r="F125" s="9" t="s">
         <v>38</v>
@@ -4134,13 +4138,13 @@
         <v>16</v>
       </c>
       <c r="C126" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D126">
-        <v>1</v>
-      </c>
-      <c r="E126">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D126" s="13">
+        <v>17</v>
+      </c>
+      <c r="E126" s="13">
+        <v>18</v>
       </c>
       <c r="F126" s="9" t="s">
         <v>38</v>
@@ -4161,13 +4165,13 @@
         <v>81</v>
       </c>
       <c r="C127" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D127">
-        <v>6</v>
-      </c>
-      <c r="E127">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D127" s="13">
+        <v>17</v>
+      </c>
+      <c r="E127" s="13">
+        <v>18</v>
       </c>
       <c r="F127" t="s">
         <v>34</v>
@@ -4188,13 +4192,13 @@
         <v>81</v>
       </c>
       <c r="C128" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D128">
-        <v>6</v>
-      </c>
-      <c r="E128">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D128" s="13">
+        <v>17</v>
+      </c>
+      <c r="E128" s="13">
+        <v>18</v>
       </c>
       <c r="F128" t="s">
         <v>34</v>
@@ -4215,13 +4219,13 @@
         <v>81</v>
       </c>
       <c r="C129" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D129">
-        <v>6</v>
-      </c>
-      <c r="E129">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D129" s="13">
+        <v>17</v>
+      </c>
+      <c r="E129" s="13">
+        <v>18</v>
       </c>
       <c r="F129" t="s">
         <v>34</v>
@@ -4242,13 +4246,13 @@
         <v>81</v>
       </c>
       <c r="C130" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D130">
-        <v>6</v>
-      </c>
-      <c r="E130">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D130" s="13">
+        <v>17</v>
+      </c>
+      <c r="E130" s="13">
+        <v>18</v>
       </c>
       <c r="F130" t="s">
         <v>39</v>
@@ -4269,13 +4273,13 @@
         <v>81</v>
       </c>
       <c r="C131" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D131">
-        <v>6</v>
-      </c>
-      <c r="E131">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D131" s="13">
+        <v>17</v>
+      </c>
+      <c r="E131" s="13">
+        <v>18</v>
       </c>
       <c r="F131" t="s">
         <v>39</v>
@@ -4296,13 +4300,13 @@
         <v>81</v>
       </c>
       <c r="C132" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D132">
-        <v>6</v>
-      </c>
-      <c r="E132">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D132" s="13">
+        <v>17</v>
+      </c>
+      <c r="E132" s="13">
+        <v>18</v>
       </c>
       <c r="F132" t="s">
         <v>35</v>
@@ -4323,13 +4327,13 @@
         <v>81</v>
       </c>
       <c r="C133" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D133">
-        <v>6</v>
-      </c>
-      <c r="E133">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D133" s="13">
+        <v>17</v>
+      </c>
+      <c r="E133" s="13">
+        <v>18</v>
       </c>
       <c r="F133" t="s">
         <v>35</v>
@@ -4350,13 +4354,13 @@
         <v>81</v>
       </c>
       <c r="C134" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D134">
-        <v>6</v>
-      </c>
-      <c r="E134">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="D134" s="13">
+        <v>17</v>
+      </c>
+      <c r="E134" s="13">
+        <v>18</v>
       </c>
       <c r="F134" t="s">
         <v>36</v>

</xml_diff>